<commit_message>
- ADD: Added set size and timeseries flag to traits/phenotypes.
</commit_message>
<xml_diff>
--- a/src/main/resources/trials-data.xlsx
+++ b/src/main/resources/trials-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\trials-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\java\gridscore-next-server\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CD3032-92FE-4E67-BDD9-F1701119FD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DC30CD-E139-412E-BB2D-98A678B171AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6570" yWindow="480" windowWidth="38700" windowHeight="15285" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="3" r:id="rId1"/>
@@ -20,10 +20,11 @@
     <sheet name="ATTRIBUTES" sheetId="11" r:id="rId5"/>
     <sheet name="COLLABORATORS" sheetId="9" r:id="rId6"/>
     <sheet name="LOCATION" sheetId="10" r:id="rId7"/>
-    <sheet name="LOCATION_EXAMPLE" sheetId="12" r:id="rId8"/>
-    <sheet name="PHENOTYPES_EXAMPLE" sheetId="5" r:id="rId9"/>
-    <sheet name="DATA_EXAMPLE" sheetId="4" r:id="rId10"/>
-    <sheet name="RECORDING_DATES_EXAMPLE" sheetId="8" r:id="rId11"/>
+    <sheet name="TYPES" sheetId="13" r:id="rId8"/>
+    <sheet name="LOCATION_EXAMPLE" sheetId="12" r:id="rId9"/>
+    <sheet name="PHENOTYPES_EXAMPLE" sheetId="5" r:id="rId10"/>
+    <sheet name="DATA_EXAMPLE" sheetId="4" r:id="rId11"/>
+    <sheet name="RECORDING_DATES_EXAMPLE" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="118">
   <si>
     <t>Name</t>
   </si>
@@ -326,9 +327,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>ValidTypes</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -405,6 +403,12 @@
   </si>
   <si>
     <t>Column</t>
+  </si>
+  <si>
+    <t>Set size</t>
+  </si>
+  <si>
+    <t>Is timeseries</t>
   </si>
 </sst>
 </file>
@@ -529,16 +533,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -550,17 +552,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -582,21 +579,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -863,6 +854,27 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:L5" totalsRowShown="0">
+  <autoFilter ref="A1:L5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Short Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Data Type"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Unit Name"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Unit Abbreviation"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Unit Descriptions"/>
+    <tableColumn id="8" xr3:uid="{4373A1C3-2A30-43A1-B715-28F976E1B901}" name="Trait categories (comma separated)"/>
+    <tableColumn id="9" xr3:uid="{1140C57E-8F80-4173-B9E2-20FEA5F07CF8}" name="Min (only for numeric traits)"/>
+    <tableColumn id="10" xr3:uid="{313A800B-A94E-4585-938C-59EE11C83AE8}" name="Max (only for numeric traits)"/>
+    <tableColumn id="11" xr3:uid="{A3C80CF4-C7CD-4FEE-B692-65A6DB7D1F67}" name="Set size"/>
+    <tableColumn id="12" xr3:uid="{06A15507-67E8-4FA2-817F-3CA3E67D6824}" name="Is timeseries"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:N12" totalsRowShown="0">
   <autoFilter ref="A1:N12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="14">
@@ -885,13 +897,15 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table44" displayName="Table44" ref="A1:K12" totalsRowShown="0">
-  <autoFilter ref="A1:K12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="11">
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table44" displayName="Table44" ref="A1:M12" totalsRowShown="0">
+  <autoFilter ref="A1:M12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Line/Phenotype"/>
     <tableColumn id="7" xr3:uid="{F56FA6B6-097B-4A91-BE3C-84316559494C}" name="Rep"/>
     <tableColumn id="8" xr3:uid="{B1199833-CBFA-4386-8BC3-8225F4549F7B}" name="Block"/>
+    <tableColumn id="13" xr3:uid="{441254E5-D6C5-45FE-B862-378E41EA89AB}" name="Row"/>
+    <tableColumn id="12" xr3:uid="{2C43E794-883F-4CC3-86B1-A954A5AD1894}" name="Column"/>
     <tableColumn id="2" xr3:uid="{372B6450-E223-4B62-BE37-A66868D227D6}" name="Treatment"/>
     <tableColumn id="5" xr3:uid="{5F0A8F5E-5F8D-498B-AA15-759C67F77D36}" name="Location"/>
     <tableColumn id="11" xr3:uid="{907497DD-05CD-436D-8F9D-C9733135B6D1}" name="Latitude"/>
@@ -906,9 +920,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDF6150C-EB7C-4511-B47B-2F8122570053}" name="Table136" displayName="Table136" ref="A1:J2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:J2" xr:uid="{4E670C69-5459-4D42-BBD4-1C0FE57A115B}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDF6150C-EB7C-4511-B47B-2F8122570053}" name="Table136" displayName="Table136" ref="A1:L2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:L2" xr:uid="{4E670C69-5459-4D42-BBD4-1C0FE57A115B}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{7A9D9CB2-5A72-4610-AB48-E51B9D320089}" name="Name"/>
     <tableColumn id="2" xr3:uid="{E96E90FF-566D-4FFD-82F1-51DBFC5414D9}" name="Short Name"/>
     <tableColumn id="3" xr3:uid="{40088974-32A7-4DF8-B510-4933C37FC25F}" name="Description"/>
@@ -919,25 +933,27 @@
     <tableColumn id="8" xr3:uid="{F0A8842E-035A-489D-85ED-9A856618A31C}" name="Trait categories (comma separated)"/>
     <tableColumn id="9" xr3:uid="{33440BAE-1141-4F5B-9E00-4E91B738E873}" name="Min (only for numeric traits)"/>
     <tableColumn id="10" xr3:uid="{3BB72CFF-4CE5-48BF-899E-D8A314EEB697}" name="Max (only for numeric traits)"/>
+    <tableColumn id="11" xr3:uid="{E6440CB8-850C-41FF-AA2B-B688CCF90613}" name="Set size"/>
+    <tableColumn id="12" xr3:uid="{55D3E326-011B-48FC-BD4F-444CBE4F0FC5}" name="Is timeseries"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{22E566EA-CF41-4BD4-A877-BF1A04CBE27C}" name="Table47" displayName="Table47" ref="A1:J2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:J2" xr:uid="{C24E8378-3794-454E-84CF-B08C2B5A27D2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EF260BCA-75E5-4914-B549-45DFEFEAB946}" name="Table6" displayName="Table6" ref="A1:J2" totalsRowShown="0">
+  <autoFilter ref="A1:J2" xr:uid="{EF260BCA-75E5-4914-B549-45DFEFEAB946}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CCD80E05-5388-423E-BBDC-2354AB7B8FC3}" name="Line/Phenotype"/>
-    <tableColumn id="2" xr3:uid="{466AEB02-1AD0-430A-B6D8-FF71A9F751B4}" name="Rep"/>
-    <tableColumn id="8" xr3:uid="{B32A4B56-1C05-4F7B-B51B-4FA3967354E2}" name="Block"/>
-    <tableColumn id="9" xr3:uid="{2ED92832-AD7D-4A22-8917-F561E101C555}" name="Row"/>
-    <tableColumn id="10" xr3:uid="{61C248C8-9EF3-432C-BE20-51527617EB5B}" name="Column"/>
-    <tableColumn id="7" xr3:uid="{40C0F606-B99C-4595-806C-A7295CC796D9}" name="Treatment"/>
-    <tableColumn id="3" xr3:uid="{8EE9A1A1-AEF3-490F-B2E4-D6A460210A54}" name="Location"/>
-    <tableColumn id="4" xr3:uid="{69C9CE63-BD11-4E4B-957D-A99D3AA2F63C}" name="Latitude"/>
-    <tableColumn id="5" xr3:uid="{67FFEBA5-AD32-417A-987A-2C040AA24764}" name="Longitude"/>
-    <tableColumn id="6" xr3:uid="{D986DFA6-2CBB-40DF-84E8-21CC5C183E1E}" name="Elevation"/>
+    <tableColumn id="1" xr3:uid="{FA206F6A-CB80-4B4B-912F-B33123820053}" name="Line/Phenotype"/>
+    <tableColumn id="2" xr3:uid="{5CA73EAD-13D2-4343-8FD5-B3663FADAB58}" name="Rep"/>
+    <tableColumn id="3" xr3:uid="{E222209F-E15B-4856-AAED-9BEBD4F891B7}" name="Block"/>
+    <tableColumn id="4" xr3:uid="{8B9B9549-197F-46BC-A29E-6D80C0A7CB3E}" name="Row"/>
+    <tableColumn id="5" xr3:uid="{E1C9DDF0-1A9A-4619-B78D-01A7ADE09403}" name="Column"/>
+    <tableColumn id="6" xr3:uid="{033FCDA4-F0DA-44BF-AA1D-716F34F95FF7}" name="Treatment"/>
+    <tableColumn id="7" xr3:uid="{A633A2C3-3081-42A7-821D-27D475BF74E4}" name="Location"/>
+    <tableColumn id="8" xr3:uid="{6AF9FB5D-6CBE-4BB5-A26B-15A3E71F843F}" name="Latitude"/>
+    <tableColumn id="9" xr3:uid="{AC696C5C-08E6-43FF-839D-DD162C848AF8}" name="Longitude"/>
+    <tableColumn id="10" xr3:uid="{115E2DAB-3E6E-46C1-835E-7FF70AFFF207}" name="Elevation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1008,6 +1024,16 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{BC0B0D73-CC3A-48CD-887A-2EF7881DDA99}" name="Table12" displayName="Table12" ref="A1:A5" totalsRowShown="0">
+  <autoFilter ref="A1:A5" xr:uid="{BC0B0D73-CC3A-48CD-887A-2EF7881DDA99}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{C0C993D3-A2AC-4650-BA96-6DDA37FE2502}" name="Possible data types"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C286F7D8-1BF5-4BEE-B3C7-5B05DC94F35F}" name="Table912" displayName="Table912" ref="A1:F3" totalsRowShown="0">
   <autoFilter ref="A1:F3" xr:uid="{AF4606A7-A239-4229-872E-C0E19378E716}"/>
   <tableColumns count="6">
@@ -1017,25 +1043,6 @@
     <tableColumn id="4" xr3:uid="{8EE06D1F-C91E-4B52-B65C-73E4021B3BA2}" name="Elevation"/>
     <tableColumn id="5" xr3:uid="{46BED72F-DD99-423F-BBBF-C7582566C178}" name="Latitude"/>
     <tableColumn id="6" xr3:uid="{625E57C8-CC0D-4812-91EC-5E30BDF78D26}" name="Longitude"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:J5" totalsRowShown="0">
-  <autoFilter ref="A1:J5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Short Name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Data Type"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Unit Name"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Unit Abbreviation"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Unit Descriptions"/>
-    <tableColumn id="8" xr3:uid="{4373A1C3-2A30-43A1-B715-28F976E1B901}" name="Trait categories (comma separated)"/>
-    <tableColumn id="9" xr3:uid="{1140C57E-8F80-4173-B9E2-20FEA5F07CF8}" name="Min (only for numeric traits)"/>
-    <tableColumn id="10" xr3:uid="{313A800B-A94E-4585-938C-59EE11C83AE8}" name="Max (only for numeric traits)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1307,224 +1314,219 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="108.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="7"/>
-    <col min="5" max="5" width="13.42578125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="108.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="5"/>
+    <col min="5" max="5" width="13.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="19"/>
+      <c r="C5" s="14"/>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="C13" s="23"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="30"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="B14" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="C14" s="23"/>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="30"/>
-    </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="B15" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="C15" s="23"/>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="30"/>
-    </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="B16" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="C16" s="23"/>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="30"/>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="B17" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="C17" s="23"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="30"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="B18" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="30"/>
+      <c r="C18" s="23"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
+      <c r="A20" s="7"/>
     </row>
     <row r="21" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="13"/>
-    </row>
-    <row r="23" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+      <c r="A22" s="7"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
+      <c r="B24" s="10"/>
     </row>
     <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>114</v>
+      <c r="B25" s="11" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="13" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1543,6 +1545,196 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="8">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Description" prompt="A description of the unit." sqref="G1" xr:uid="{16D5CC04-3B65-4F55-B2C4-EE9D936D07C4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Abbreviation" prompt="Abbreviation for unit. Examples include 'l' or 'cm'" sqref="F1" xr:uid="{AC4F8502-A851-4CCB-B918-5D4763FB006B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Name" prompt="The name of the unit that is defined. Examples would include 'centimetre' or 'litre'" sqref="E1" xr:uid="{37849AFC-2B54-4F44-9627-B74E742F0D18}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Description" prompt="This should be a full description of the phenotype. There is no limit to the length of text that can be used here so please be descriptive." sqref="C1" xr:uid="{2CCAF288-83B4-472D-98B9-8B258E2B4286}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Short Name" prompt="This is should be a shortened version of the phenotype name. This is used on some of the Germinate pages which use tables so that the phenotype name fits." sqref="B1" xr:uid="{FAAEA96D-BB37-46C4-B5FE-E1B1136C836A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Name" prompt="This should be the full name of the phenotype that has been scored." sqref="A1" xr:uid="{08E60448-4E9F-47ED-930C-AB529B5A231D}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{9D8AB10C-6262-46B1-9E10-D45C03C4CFD6}">
+      <formula1>$L$2:$L$4</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Trait categories" prompt="These are the possible values of this trait. Please specify them in this format_x000a_[[&quot;first&quot;, &quot;second&quot;, &quot;third&quot;],[&quot;1&quot;, &quot;2&quot;, &quot;3&quot;]]_x000a_This example shows two scales for this trait, one descriptive and one numerical. If you only have one, please only specify one." sqref="H1" xr:uid="{27E89C82-A161-4A20-A11B-D2A61F76957B}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -1550,18 +1742,18 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D1" sqref="D1:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="6.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -1569,426 +1761,424 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2">
         <v>56.46152</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2">
         <v>-3.1109200000000001</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2">
         <v>38.9</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2">
         <v>15.698600000000001</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2">
         <v>7</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2">
         <v>20.435199999999998</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3">
         <v>56.470471000000003</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3">
         <v>-3.1227999999999998</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3">
         <v>26.4</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3">
         <v>17.075500000000002</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3">
         <v>8</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3">
         <v>24.342500000000001</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="4">
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4">
         <v>56.465794000000002</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4">
         <v>-3.12696</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4">
         <v>98.1</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4">
         <v>5.6565000000000003</v>
       </c>
-      <c r="L4" s="4">
-        <v>1</v>
-      </c>
-      <c r="M4" s="4">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>10.432399999999999</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" s="4">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="G5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5">
         <v>56.468415</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5">
         <v>-3.1256499999999998</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5">
         <v>76.5</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5">
         <v>6.4452999999999996</v>
       </c>
-      <c r="L5" s="4">
-        <v>2</v>
-      </c>
-      <c r="M5" s="4">
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
         <v>9.4054000000000002</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6">
         <v>56.470269999999999</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6">
         <v>-3.1406999999999998</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6">
         <v>76.2</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6">
         <v>16.232500000000002</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4">
+      <c r="M6">
         <v>21.435600000000001</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="4">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4">
-        <v>2</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="G7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7">
         <v>56.471969000000001</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7">
         <v>-3.11985</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7">
         <v>62.4</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7">
         <v>17.552600000000002</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4">
+      <c r="M7">
         <v>22.467400000000001</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
         <v>3</v>
       </c>
-      <c r="E8" s="4">
-        <v>2</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="G8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8">
         <v>56.468760000000003</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8">
         <v>-3.1153</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8">
         <v>56.4</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8">
         <v>4.5321999999999996</v>
       </c>
-      <c r="L8" s="4">
-        <v>2</v>
-      </c>
-      <c r="M8" s="4">
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
         <v>16.546600000000002</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="4">
-        <v>2</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <v>4</v>
       </c>
-      <c r="E9" s="4">
-        <v>2</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="G9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9">
         <v>56.467841999999997</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9">
         <v>-3.1088</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9">
         <v>68.900000000000006</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9">
         <v>6.3562000000000003</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9">
         <v>3</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9">
         <v>15.545299999999999</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
         <v>3</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="G10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10">
         <v>56.469270999999999</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10">
         <v>-3.14317</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10">
         <v>85.6</v>
       </c>
       <c r="K10">
@@ -2000,39 +2190,39 @@
       <c r="M10">
         <v>24.545300000000001</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="N10" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="4">
-        <v>2</v>
-      </c>
-      <c r="C11" s="4">
-        <v>2</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
         <v>3</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11">
         <v>56.472653000000001</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11">
         <v>-3.1432699999999998</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11">
         <v>23.6</v>
       </c>
       <c r="K11">
@@ -2044,39 +2234,39 @@
       <c r="M11">
         <v>25.5366</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N11" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
         <v>3</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12">
         <v>3</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H12" s="4">
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12">
         <v>56.461801000000001</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12">
         <v>-3.1385399999999999</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12">
         <v>85.9</v>
       </c>
       <c r="L12">
@@ -2085,7 +2275,7 @@
       <c r="M12">
         <v>9.4344999999999999</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="N12" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2098,479 +2288,550 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="12.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="H2">
+        <v>56.46152</v>
+      </c>
+      <c r="I2">
+        <v>-3.1109200000000001</v>
+      </c>
+      <c r="J2">
+        <v>38.9</v>
+      </c>
+      <c r="K2" s="3">
+        <v>42371</v>
+      </c>
+      <c r="L2" s="3">
+        <v>42373</v>
+      </c>
+      <c r="M2" s="3">
+        <v>42373</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" s="4">
-        <v>56.46152</v>
-      </c>
-      <c r="G2" s="4">
-        <v>-3.1109200000000001</v>
-      </c>
-      <c r="H2" s="4">
-        <v>38.9</v>
-      </c>
-      <c r="I2" s="5">
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3">
+        <v>56.470471000000003</v>
+      </c>
+      <c r="I3">
+        <v>-3.1227999999999998</v>
+      </c>
+      <c r="J3">
+        <v>26.4</v>
+      </c>
+      <c r="K3" s="3">
+        <v>42370</v>
+      </c>
+      <c r="L3" s="3">
+        <v>42375</v>
+      </c>
+      <c r="M3" s="3">
+        <v>42370</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4">
+        <v>56.465794000000002</v>
+      </c>
+      <c r="I4">
+        <v>-3.12696</v>
+      </c>
+      <c r="J4">
+        <v>98.1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>42377</v>
+      </c>
+      <c r="L4" s="3">
+        <v>42372</v>
+      </c>
+      <c r="M4" s="3">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5">
+        <v>56.468415</v>
+      </c>
+      <c r="I5">
+        <v>-3.1256499999999998</v>
+      </c>
+      <c r="J5">
+        <v>76.5</v>
+      </c>
+      <c r="K5" s="3">
+        <v>42378</v>
+      </c>
+      <c r="L5" s="3">
+        <v>42377</v>
+      </c>
+      <c r="M5" s="3">
+        <v>42374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6">
+        <v>56.470269999999999</v>
+      </c>
+      <c r="I6">
+        <v>-3.1406999999999998</v>
+      </c>
+      <c r="J6">
+        <v>76.2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>42376</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3">
+        <v>42373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7">
+        <v>56.471969000000001</v>
+      </c>
+      <c r="I7">
+        <v>-3.11985</v>
+      </c>
+      <c r="J7">
+        <v>62.4</v>
+      </c>
+      <c r="K7" s="3">
+        <v>42374</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3">
+        <v>42375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8">
+        <v>56.468760000000003</v>
+      </c>
+      <c r="I8">
+        <v>-3.1153</v>
+      </c>
+      <c r="J8">
+        <v>56.4</v>
+      </c>
+      <c r="K8" s="3">
         <v>42371</v>
       </c>
-      <c r="J2" s="5">
+      <c r="L8" s="3">
+        <v>42374</v>
+      </c>
+      <c r="M8" s="3">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9">
+        <v>56.467841999999997</v>
+      </c>
+      <c r="I9">
+        <v>-3.1088</v>
+      </c>
+      <c r="J9">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="K9" s="3">
+        <v>42379</v>
+      </c>
+      <c r="L9" s="3">
+        <v>42376</v>
+      </c>
+      <c r="M9" s="3">
         <v>42373</v>
       </c>
-      <c r="K2" s="5">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10">
+        <v>56.469270999999999</v>
+      </c>
+      <c r="I10">
+        <v>-3.14317</v>
+      </c>
+      <c r="J10">
+        <v>85.6</v>
+      </c>
+      <c r="K10" s="3">
         <v>42373</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="L10" s="3">
+        <v>42374</v>
+      </c>
+      <c r="M10" s="3">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="4">
-        <v>56.470471000000003</v>
-      </c>
-      <c r="G3" s="4">
-        <v>-3.1227999999999998</v>
-      </c>
-      <c r="H3" s="4">
-        <v>26.4</v>
-      </c>
-      <c r="I3" s="5">
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11">
+        <v>56.472653000000001</v>
+      </c>
+      <c r="I11">
+        <v>-3.1432699999999998</v>
+      </c>
+      <c r="J11">
+        <v>23.6</v>
+      </c>
+      <c r="K11" s="3">
+        <v>42379</v>
+      </c>
+      <c r="L11" s="3">
+        <v>42376</v>
+      </c>
+      <c r="M11" s="3">
+        <v>42374</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12">
+        <v>56.461801000000001</v>
+      </c>
+      <c r="I12">
+        <v>-3.1385399999999999</v>
+      </c>
+      <c r="J12">
+        <v>85.9</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3">
         <v>42370</v>
       </c>
-      <c r="J3" s="5">
-        <v>42375</v>
-      </c>
-      <c r="K3" s="5">
-        <v>42370</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" s="4">
-        <v>56.465794000000002</v>
-      </c>
-      <c r="G4" s="4">
-        <v>-3.12696</v>
-      </c>
-      <c r="H4" s="4">
-        <v>98.1</v>
-      </c>
-      <c r="I4" s="5">
-        <v>42377</v>
-      </c>
-      <c r="J4" s="5">
+      <c r="M12" s="3">
         <v>42372</v>
       </c>
-      <c r="K4" s="5">
-        <v>42377</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="4">
-        <v>56.468415</v>
-      </c>
-      <c r="G5" s="4">
-        <v>-3.1256499999999998</v>
-      </c>
-      <c r="H5" s="4">
-        <v>76.5</v>
-      </c>
-      <c r="I5" s="5">
-        <v>42378</v>
-      </c>
-      <c r="J5" s="5">
-        <v>42377</v>
-      </c>
-      <c r="K5" s="5">
-        <v>42374</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F6" s="4">
-        <v>56.470269999999999</v>
-      </c>
-      <c r="G6" s="4">
-        <v>-3.1406999999999998</v>
-      </c>
-      <c r="H6" s="4">
-        <v>76.2</v>
-      </c>
-      <c r="I6" s="5">
-        <v>42376</v>
-      </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5">
-        <v>42373</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="4">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="4">
-        <v>56.471969000000001</v>
-      </c>
-      <c r="G7" s="4">
-        <v>-3.11985</v>
-      </c>
-      <c r="H7" s="4">
-        <v>62.4</v>
-      </c>
-      <c r="I7" s="5">
-        <v>42374</v>
-      </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5">
-        <v>42375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8" s="4">
-        <v>56.468760000000003</v>
-      </c>
-      <c r="G8" s="4">
-        <v>-3.1153</v>
-      </c>
-      <c r="H8" s="4">
-        <v>56.4</v>
-      </c>
-      <c r="I8" s="5">
-        <v>42371</v>
-      </c>
-      <c r="J8" s="5">
-        <v>42374</v>
-      </c>
-      <c r="K8" s="5">
-        <v>42376</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="4">
-        <v>2</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="4">
-        <v>56.467841999999997</v>
-      </c>
-      <c r="G9" s="4">
-        <v>-3.1088</v>
-      </c>
-      <c r="H9" s="4">
-        <v>68.900000000000006</v>
-      </c>
-      <c r="I9" s="5">
-        <v>42379</v>
-      </c>
-      <c r="J9" s="5">
-        <v>42376</v>
-      </c>
-      <c r="K9" s="5">
-        <v>42373</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10" s="4">
-        <v>56.469270999999999</v>
-      </c>
-      <c r="G10" s="4">
-        <v>-3.14317</v>
-      </c>
-      <c r="H10" s="4">
-        <v>85.6</v>
-      </c>
-      <c r="I10" s="5">
-        <v>42373</v>
-      </c>
-      <c r="J10" s="5">
-        <v>42374</v>
-      </c>
-      <c r="K10" s="5">
-        <v>42376</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="4">
-        <v>2</v>
-      </c>
-      <c r="C11" s="4">
-        <v>2</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="4">
-        <v>56.472653000000001</v>
-      </c>
-      <c r="G11" s="4">
-        <v>-3.1432699999999998</v>
-      </c>
-      <c r="H11" s="4">
-        <v>23.6</v>
-      </c>
-      <c r="I11" s="5">
-        <v>42379</v>
-      </c>
-      <c r="J11" s="5">
-        <v>42376</v>
-      </c>
-      <c r="K11" s="5">
-        <v>42374</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F12" s="4">
-        <v>56.461801000000001</v>
-      </c>
-      <c r="G12" s="4">
-        <v>-3.1385399999999999</v>
-      </c>
-      <c r="H12" s="4">
-        <v>85.9</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5">
-        <v>42370</v>
-      </c>
-      <c r="K12" s="5">
-        <v>42372</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I19" s="5"/>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="J20" s="5"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K19" s="3"/>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1:H1" xr:uid="{00000000-0002-0000-0600-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1:J1" xr:uid="{00000000-0002-0000-0600-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -2582,10 +2843,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L5"/>
+      <selection activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2599,85 +2860,47 @@
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="4"/>
-    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="26" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" t="s">
         <v>78</v>
       </c>
+      <c r="K1" t="s">
+        <v>116</v>
+      </c>
       <c r="L1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="L2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="L3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="L4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L5" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2686,42 +2909,48 @@
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="8">
+  <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Name" prompt="This should be the full name of the phenotype that has been scored." sqref="A1" xr:uid="{53C12F0B-3F9F-48BF-B0F0-E08B964BA4CC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Short Name" prompt="This is should be a shortened version of the phenotype name. This is used on some of the Germinate pages which use tables so that the phenotype name fits." sqref="B1" xr:uid="{8C19ED97-A603-4BB6-A206-2A716846C37F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Description" prompt="This should be a full description of the phenotype. There is no limit to the length of text that can be used here so please be descriptive." sqref="C1" xr:uid="{F089AE66-013F-4735-81BE-5882571D1849}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Name" prompt="The name of the unit that is defined. Examples would include 'centimetre' or 'litre'" sqref="E1" xr:uid="{812908F9-58E0-44B7-8D9B-8F24F8373A14}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Abbreviation" prompt="Abbreviation for unit. Examples include 'l' or 'cm'" sqref="F1" xr:uid="{240F401A-C0EB-48A0-9B93-B4062FF9E866}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Description" prompt="A description of the unit." sqref="G1" xr:uid="{6BD03C10-201D-4FCC-A927-CC3E06375029}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D3:D1048576" xr:uid="{82E3529B-0246-482A-A1C4-DA13B1AEE9F4}">
-      <formula1>$L$2:$L$4</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{E7F82065-00E0-406C-B1D1-FF1C0CCD1326}">
-      <formula1>$L$2:$L$5</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E7F82065-00E0-406C-B1D1-FF1C0CCD1326}">
+          <x14:formula1>
+            <xm:f>TYPES!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -2730,26 +2959,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H1" t="s">
         <v>71</v>
@@ -2761,67 +2990,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Lines (ACCENUMB from MCPD data) on the Y axis and phenotypes (which are described in PHENOTYPES tab) on the x axis. The actual phenotype value goes in the matrix cells. See DATA_EXAMPLE tab for more information before completion." sqref="A1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
   </dataValidations>
@@ -2835,7 +3004,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -2845,9 +3014,9 @@
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -2856,26 +3025,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H1" t="s">
         <v>71</v>
@@ -2886,11 +3055,6 @@
       <c r="J1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="F2" s="4"/>
     </row>
   </sheetData>
   <dataValidations xWindow="96" yWindow="450" count="1">
@@ -2905,63 +3069,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829331A2-8F6C-4EC4-B723-84C59F96FDF0}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>44</v>
       </c>
       <c r="C1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H2" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H3" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H4" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H5" s="4" t="s">
-        <v>76</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{A99E7B79-269E-427E-A290-9658276FC0EE}">
-      <formula1>$H$2:$H$5</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A99E7B79-269E-427E-A290-9658276FC0EE}">
+          <x14:formula1>
+            <xm:f>TYPES!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2975,71 +3123,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" style="22" customWidth="1"/>
-    <col min="2" max="4" width="40.85546875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="46.42578125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="53.140625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="25" style="22" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="22" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="42.42578125" style="17" customWidth="1"/>
+    <col min="2" max="4" width="40.85546875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="53.140625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="17" customWidth="1"/>
+    <col min="8" max="8" width="25" style="17" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="29" t="s">
+      <c r="D2" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="15" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3103,11 +3251,57 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA6958C-AADA-494D-9D10-2CEB6E18F22F}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F59A9259-3A2D-497C-B3D7-300C547C2DDB}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:F3"/>
@@ -3116,88 +3310,64 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>56.483783000000003</v>
+      </c>
+      <c r="F2">
+        <v>-3.1135030000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="4">
-        <v>30</v>
-      </c>
-      <c r="E2" s="4">
-        <v>56.483783000000003</v>
-      </c>
-      <c r="F2" s="4">
-        <v>-3.1135030000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B3" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3">
         <v>140</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3">
         <v>56.481081000000003</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3">
         <v>-3.135132</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3209,167 +3379,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="104.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Description" prompt="A description of the unit." sqref="G1" xr:uid="{16D5CC04-3B65-4F55-B2C4-EE9D936D07C4}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Abbreviation" prompt="Abbreviation for unit. Examples include 'l' or 'cm'" sqref="F1" xr:uid="{AC4F8502-A851-4CCB-B918-5D4763FB006B}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Name" prompt="The name of the unit that is defined. Examples would include 'centimetre' or 'litre'" sqref="E1" xr:uid="{37849AFC-2B54-4F44-9627-B74E742F0D18}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Description" prompt="This should be a full description of the phenotype. There is no limit to the length of text that can be used here so please be descriptive." sqref="C1" xr:uid="{2CCAF288-83B4-472D-98B9-8B258E2B4286}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Short Name" prompt="This is should be a shortened version of the phenotype name. This is used on some of the Germinate pages which use tables so that the phenotype name fits." sqref="B1" xr:uid="{FAAEA96D-BB37-46C4-B5FE-E1B1136C836A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Name" prompt="This should be the full name of the phenotype that has been scored." sqref="A1" xr:uid="{08E60448-4E9F-47ED-930C-AB529B5A231D}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{9D8AB10C-6262-46B1-9E10-D45C03C4CFD6}">
-      <formula1>$L$2:$L$4</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Trait categories" prompt="These are the possible values of this trait. Please specify them in this format_x000a_[[&quot;first&quot;, &quot;second&quot;, &quot;third&quot;],[&quot;1&quot;, &quot;2&quot;, &quot;3&quot;]]_x000a_This example shows two scales for this trait, one descriptive and one numerical. If you only have one, please only specify one." sqref="H1" xr:uid="{27E89C82-A161-4A20-A11B-D2A61F76957B}"/>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- ADD: Added handling for trial groups during synchronization. - ADD: Added new columns to Germinate template export. -
</commit_message>
<xml_diff>
--- a/src/main/resources/trials-data.xlsx
+++ b/src/main/resources/trials-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\java\gridscore-next-server\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DC30CD-E139-412E-BB2D-98A678B171AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D3DE7B-D7CA-4DE4-ABCE-5C704B3A811E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="480" windowWidth="38700" windowHeight="15285" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46050" yWindow="2850" windowWidth="28800" windowHeight="15225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="119">
   <si>
     <t>Name</t>
   </si>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t>Is timeseries</t>
+  </si>
+  <si>
+    <t>Trait category</t>
   </si>
 </sst>
 </file>
@@ -602,14 +605,7 @@
     <cellStyle name="Normal 4" xfId="1" xr:uid="{AC6FD0CA-C916-4E1F-8927-7A9CF5AB4487}"/>
     <cellStyle name="Warning Text" xfId="3" builtinId="11"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <fill>
         <patternFill>
@@ -826,8 +822,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="26"/>
-      <tableStyleElement type="headerRow" dxfId="25"/>
+      <tableStyleElement type="wholeTable" dxfId="25"/>
+      <tableStyleElement type="headerRow" dxfId="24"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -842,12 +838,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFAA9A6-0123-422D-B80F-81EB2270DAA0}" name="Table7" displayName="Table7" ref="A1:C18" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFAA9A6-0123-422D-B80F-81EB2270DAA0}" name="Table7" displayName="Table7" ref="A1:C18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:C18" xr:uid="{DCA4608A-E2D9-45F1-81E3-F49396F38526}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1E03C996-7263-422B-8AA0-13669C78161F}" name="LABEL" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{A20F043F-90CD-41BB-866B-522B95F3EC18}" name="DEFINITION" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{139364FF-5D24-40BF-A84C-CF209A3E5D65}" name="VALUE" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{1E03C996-7263-422B-8AA0-13669C78161F}" name="LABEL" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{A20F043F-90CD-41BB-866B-522B95F3EC18}" name="DEFINITION" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{139364FF-5D24-40BF-A84C-CF209A3E5D65}" name="VALUE" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -885,9 +881,9 @@
     <tableColumn id="14" xr3:uid="{CE255CEA-3127-418C-9432-3F63F51FD781}" name="Column"/>
     <tableColumn id="7" xr3:uid="{88B30358-C3FE-4E11-B08D-42FB21CD6479}" name="Treatment"/>
     <tableColumn id="8" xr3:uid="{13CC7C54-6C19-41EF-BA0D-75E84678E993}" name="Location"/>
-    <tableColumn id="10" xr3:uid="{4DB6F789-093F-4C73-B982-C2E54070E165}" name="Latitude" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{7DF6B222-3988-4F46-991B-F6C2F213B41D}" name="Longitude" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{55ED41BA-9315-4A55-B989-C3614B9C3340}" name="Elevation" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{4DB6F789-093F-4C73-B982-C2E54070E165}" name="Latitude" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{7DF6B222-3988-4F46-991B-F6C2F213B41D}" name="Longitude" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{55ED41BA-9315-4A55-B989-C3614B9C3340}" name="Elevation" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Ear length"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Ear number per plant"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Ear width"/>
@@ -911,18 +907,18 @@
     <tableColumn id="11" xr3:uid="{907497DD-05CD-436D-8F9D-C9733135B6D1}" name="Latitude"/>
     <tableColumn id="10" xr3:uid="{F68843F4-17C8-471E-8FEA-8A1CF9BD7F9F}" name="Longitude"/>
     <tableColumn id="9" xr3:uid="{97B62C49-64CB-4474-93B9-41298499FF28}" name="Elevation"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Ear length" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Ear number per plant" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Ear width" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Ear length" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Ear number per plant" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Ear width" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDF6150C-EB7C-4511-B47B-2F8122570053}" name="Table136" displayName="Table136" ref="A1:L2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:L2" xr:uid="{4E670C69-5459-4D42-BBD4-1C0FE57A115B}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDF6150C-EB7C-4511-B47B-2F8122570053}" name="Table136" displayName="Table136" ref="A1:M2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:M2" xr:uid="{4E670C69-5459-4D42-BBD4-1C0FE57A115B}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{7A9D9CB2-5A72-4610-AB48-E51B9D320089}" name="Name"/>
     <tableColumn id="2" xr3:uid="{E96E90FF-566D-4FFD-82F1-51DBFC5414D9}" name="Short Name"/>
     <tableColumn id="3" xr3:uid="{40088974-32A7-4DF8-B510-4933C37FC25F}" name="Description"/>
@@ -935,6 +931,7 @@
     <tableColumn id="10" xr3:uid="{3BB72CFF-4CE5-48BF-899E-D8A314EEB697}" name="Max (only for numeric traits)"/>
     <tableColumn id="11" xr3:uid="{E6440CB8-850C-41FF-AA2B-B688CCF90613}" name="Set size"/>
     <tableColumn id="12" xr3:uid="{55D3E326-011B-48FC-BD4F-444CBE4F0FC5}" name="Is timeseries"/>
+    <tableColumn id="13" xr3:uid="{DE88BD84-2A95-4073-BC3E-2A52432A68E6}" name="Trait category"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -991,18 +988,18 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:I2" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:I2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:I2" xr:uid="{1B38FBA2-DC2A-4EE8-9782-869C402F129F}"/>
   <tableColumns count="9">
-    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{B35B0A33-6132-493B-9131-6BA92C731A13}" name="Contributor role" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{901F3798-43D3-40F0-8C23-0793303EE87C}" name="Contributor ID" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="10"/>
-    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{B35B0A33-6132-493B-9131-6BA92C731A13}" name="Contributor role" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{901F3798-43D3-40F0-8C23-0793303EE87C}" name="Contributor ID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1317,18 +1314,18 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="108.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="5"/>
-    <col min="5" max="5" width="13.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="22.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.453125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="108.26953125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="5"/>
+    <col min="5" max="5" width="13.453125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -1339,7 +1336,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>36</v>
       </c>
@@ -1348,7 +1345,7 @@
       </c>
       <c r="C2" s="7"/>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
@@ -1357,7 +1354,7 @@
       </c>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>37</v>
       </c>
@@ -1366,7 +1363,7 @@
       </c>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
@@ -1375,7 +1372,7 @@
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>39</v>
       </c>
@@ -1384,7 +1381,7 @@
       </c>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
@@ -1393,7 +1390,7 @@
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>42</v>
       </c>
@@ -1402,7 +1399,7 @@
       </c>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>43</v>
       </c>
@@ -1411,7 +1408,7 @@
       </c>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
@@ -1420,7 +1417,7 @@
       </c>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>53</v>
       </c>
@@ -1429,7 +1426,7 @@
       </c>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
@@ -1438,7 +1435,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>97</v>
       </c>
@@ -1447,7 +1444,7 @@
       </c>
       <c r="C13" s="23"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
         <v>99</v>
       </c>
@@ -1456,7 +1453,7 @@
       </c>
       <c r="C14" s="23"/>
     </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
         <v>101</v>
       </c>
@@ -1465,7 +1462,7 @@
       </c>
       <c r="C15" s="23"/>
     </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
         <v>103</v>
       </c>
@@ -1474,7 +1471,7 @@
       </c>
       <c r="C16" s="23"/>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
         <v>105</v>
       </c>
@@ -1483,7 +1480,7 @@
       </c>
       <c r="C17" s="23"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
         <v>107</v>
       </c>
@@ -1492,15 +1489,15 @@
       </c>
       <c r="C18" s="23"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
@@ -1508,13 +1505,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="24" t="s">
         <v>11</v>
       </c>
@@ -1522,7 +1519,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>12</v>
       </c>
@@ -1532,7 +1529,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1555,21 +1552,21 @@
       <selection activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="104.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1607,7 +1604,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1636,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1662,7 +1659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1691,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -1745,22 +1742,22 @@
       <selection activeCell="D1" sqref="D1:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="6.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="6.7265625" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.54296875" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1804,7 +1801,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1848,7 +1845,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1892,7 +1889,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1936,7 +1933,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1980,7 +1977,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2021,7 +2018,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2062,7 +2059,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2106,7 +2103,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2150,7 +2147,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2194,7 +2191,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2238,7 +2235,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -2299,19 +2296,19 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="6.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="6.7265625" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="12.54296875" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2352,7 +2349,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2393,7 +2390,7 @@
         <v>42373</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2434,7 +2431,7 @@
         <v>42370</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2475,7 +2472,7 @@
         <v>42377</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2516,7 +2513,7 @@
         <v>42374</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2555,7 +2552,7 @@
         <v>42373</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2594,7 +2591,7 @@
         <v>42375</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2635,7 +2632,7 @@
         <v>42376</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2676,7 +2673,7 @@
         <v>42373</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2717,7 +2714,7 @@
         <v>42376</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2758,7 +2755,7 @@
         <v>42374</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -2797,36 +2794,36 @@
         <v>42372</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:13" x14ac:dyDescent="0.35">
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:13" x14ac:dyDescent="0.35">
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="11:13" x14ac:dyDescent="0.35">
       <c r="K19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="11:13" x14ac:dyDescent="0.35">
       <c r="L20" s="3"/>
     </row>
   </sheetData>
@@ -2843,29 +2840,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2902,10 +2899,13 @@
       <c r="L1" t="s">
         <v>117</v>
       </c>
+      <c r="M1" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2 D2">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2940,25 +2940,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -3010,21 +3010,21 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -3075,14 +3075,14 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -3121,19 +3121,19 @@
       <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" style="17" customWidth="1"/>
-    <col min="2" max="4" width="40.85546875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="46.42578125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="53.140625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="42.453125" style="17" customWidth="1"/>
+    <col min="2" max="4" width="40.81640625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="46.453125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="53.1796875" style="18" customWidth="1"/>
+    <col min="7" max="7" width="42.26953125" style="17" customWidth="1"/>
     <col min="8" max="8" width="25" style="17" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="17" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="17"/>
+    <col min="9" max="9" width="13.453125" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>56</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>61</v>
       </c>
@@ -3208,17 +3208,17 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3258,32 +3258,32 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -3307,9 +3307,9 @@
       <selection activeCell="E2" sqref="E2:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>-3.1135030000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>94</v>
       </c>

</xml_diff>